<commit_message>
#355 nested sctruct implemented
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982F8CA1-DD73-469E-98B6-28ECB4DFEA95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0588A7-AF42-4835-BAC5-0EFB50B176D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3390" windowWidth="20580" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="16457" windowHeight="8743" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWithDoc" sheetId="3" r:id="rId1"/>
     <sheet name="Stringfields-Seq" sheetId="2" r:id="rId2"/>
     <sheet name="Stringfields-All" sheetId="4" r:id="rId3"/>
+    <sheet name="NestedStructure" sheetId="5" r:id="rId4"/>
+    <sheet name="StructureOrder" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -64,6 +66,36 @@
   </si>
   <si>
     <t>Stringfields-All</t>
+  </si>
+  <si>
+    <t>NestedStructure</t>
+  </si>
+  <si>
+    <t>stringField11</t>
+  </si>
+  <si>
+    <t>SubStruct</t>
+  </si>
+  <si>
+    <t>multiplicity</t>
+  </si>
+  <si>
+    <t>0..*</t>
+  </si>
+  <si>
+    <t>StructureOrder</t>
+  </si>
+  <si>
+    <t>SubStruct1</t>
+  </si>
+  <si>
+    <t>SubStruct2</t>
+  </si>
+  <si>
+    <t>stringField21</t>
+  </si>
+  <si>
+    <t>stringField3</t>
   </si>
 </sst>
 </file>
@@ -933,19 +965,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6C6293-5B1C-4F89-BC4D-0A9ED1B670C5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" customWidth="1"/>
+    <col min="3" max="3" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.3828125" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -956,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -980,16 +1012,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="13.3828125" customWidth="1"/>
+    <col min="5" max="5" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1003,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1051,18 +1083,18 @@
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1092,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1101,6 +1133,223 @@
       </c>
       <c r="C4" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922B866E-1790-4F0D-A46D-71DD363647DD}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CEEB4F-74FB-492B-90A7-3FBAFE27B880}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.3828125" customWidth="1"/>
+    <col min="5" max="5" width="17.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#355 basic attribute generation works
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0588A7-AF42-4835-BAC5-0EFB50B176D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C172BCD1-46E5-40BC-89D2-1A1184752D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="377" yWindow="377" windowWidth="16457" windowHeight="8743" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="16457" windowHeight="8743" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWithDoc" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Stringfields-All" sheetId="4" r:id="rId3"/>
     <sheet name="NestedStructure" sheetId="5" r:id="rId4"/>
     <sheet name="StructureOrder" sheetId="6" r:id="rId5"/>
+    <sheet name="Attribute" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -96,6 +97,18 @@
   </si>
   <si>
     <t>stringField3</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>stringAttr1</t>
+  </si>
+  <si>
+    <t>stringAttr2</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CEEB4F-74FB-492B-90A7-3FBAFE27B880}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -1356,4 +1369,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFAF72-E3D7-4B54-B2DD-F3D1F80B1514}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="16.84375" customWidth="1"/>
+    <col min="4" max="4" width="15.3828125" customWidth="1"/>
+    <col min="5" max="5" width="12.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
355 complex PatientDetails example
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C172BCD1-46E5-40BC-89D2-1A1184752D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7ED914-B18D-4750-A55D-A07AE645FD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="377" yWindow="377" windowWidth="16457" windowHeight="8743" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWithDoc" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="NestedStructure" sheetId="5" r:id="rId4"/>
     <sheet name="StructureOrder" sheetId="6" r:id="rId5"/>
     <sheet name="Attribute" sheetId="7" r:id="rId6"/>
+    <sheet name="PatientDetails" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -109,6 +110,57 @@
   </si>
   <si>
     <t>stringAttr2</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>InsuranceNumber</t>
+  </si>
+  <si>
+    <t>123456789ABC</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>This is the Schema for Basic Tutorial</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>DateOfBirth docs</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>male, female</t>
+  </si>
+  <si>
+    <t>unit.values</t>
+  </si>
+  <si>
+    <t>unit.default</t>
+  </si>
+  <si>
+    <t>g, kg</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>PatientDetails</t>
   </si>
 </sst>
 </file>
@@ -618,9 +670,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1375,7 +1428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFAF72-E3D7-4B54-B2DD-F3D1F80B1514}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1421,4 +1474,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70417D87-787B-45F4-B2D5-D627C1744BF7}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="16.4609375" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" customWidth="1"/>
+    <col min="4" max="4" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.921875" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" customWidth="1"/>
+    <col min="7" max="7" width="12.53515625" customWidth="1"/>
+    <col min="8" max="8" width="15.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#355 ExcelGroovyParser multi-line header with merged cells
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7ED914-B18D-4750-A55D-A07AE645FD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62226F18-9377-4704-A83A-D33A3B9FCBAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="25440" windowHeight="15540" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWithDoc" sheetId="3" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="StructureOrder" sheetId="6" r:id="rId5"/>
     <sheet name="Attribute" sheetId="7" r:id="rId6"/>
     <sheet name="PatientDetails" sheetId="9" r:id="rId7"/>
+    <sheet name="PatientDetailsEnhanced" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -161,13 +162,22 @@
   </si>
   <si>
     <t>PatientDetails</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>PatientDetailsEnhanced</t>
+  </si>
+  <si>
+    <t>schema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,8 +338,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,8 +536,38 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -625,6 +682,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -670,10 +871,52 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1035,15 +1278,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.84375" customWidth="1"/>
-    <col min="3" max="3" width="28.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3828125" customWidth="1"/>
-    <col min="6" max="6" width="12.53515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1078,16 +1321,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="15.15234375" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" customWidth="1"/>
-    <col min="4" max="4" width="13.3828125" customWidth="1"/>
-    <col min="5" max="5" width="17.69140625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1101,7 +1344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1112,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1149,18 +1392,18 @@
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" customWidth="1"/>
-    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" customWidth="1"/>
-    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1171,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1190,7 +1433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1216,18 +1459,18 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3046875" customWidth="1"/>
-    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" customWidth="1"/>
-    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1241,7 +1484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1252,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1313,16 +1556,16 @@
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.3828125" customWidth="1"/>
-    <col min="5" max="5" width="17.69140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1338,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1346,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1378,7 +1621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1394,7 +1637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1432,14 +1675,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.84375" customWidth="1"/>
-    <col min="4" max="4" width="15.3828125" customWidth="1"/>
-    <col min="5" max="5" width="12.53515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1463,7 +1706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1480,120 +1723,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70417D87-787B-45F4-B2D5-D627C1744BF7}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="16.4609375" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" customWidth="1"/>
-    <col min="4" max="4" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.921875" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" customWidth="1"/>
-    <col min="7" max="7" width="12.53515625" customWidth="1"/>
-    <col min="8" max="8" width="15.69140625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="H6" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1933C8D2-90B5-4905-8E5A-4143FA2B0F50}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#355 extended complex example
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderStruct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE5FC34-B59B-4B48-839F-63B4C4763B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABACEE2-3C9C-4ABC-BCC6-6E667DC288CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWithDoc" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -161,6 +161,33 @@
   </si>
   <si>
     <t>xsd</t>
+  </si>
+  <si>
+    <t>dynamicForms</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>999.99</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>updateScriptRef</t>
+  </si>
+  <si>
+    <t>Script:0</t>
+  </si>
+  <si>
+    <t>FullName</t>
   </si>
 </sst>
 </file>
@@ -341,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,8 +578,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -811,6 +850,43 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -864,7 +940,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -879,7 +955,6 @@
     <xf numFmtId="0" fontId="18" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,12 +962,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,6 +973,15 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -913,9 +991,15 @@
     <xf numFmtId="0" fontId="18" fillId="36" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="39" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1274,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6C6293-5B1C-4F89-BC4D-0A9ED1B670C5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1287,11 +1371,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1341,12 +1425,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1425,11 +1509,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1502,12 +1586,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1608,10 +1692,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1734,10 +1818,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -1781,25 +1865,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1933C8D2-90B5-4905-8E5A-4143FA2B0F50}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11.84375" style="4" customWidth="1"/>
     <col min="2" max="2" width="24.3046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" style="16" customWidth="1"/>
     <col min="4" max="4" width="13.3046875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.69140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.3046875" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.15234375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.53515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.53515625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="14.23046875" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23046875" style="29"/>
+    <col min="12" max="12" width="14.3046875" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.23046875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
         <v>44</v>
       </c>
@@ -1808,19 +1896,26 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="25"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H1" s="22"/>
+      <c r="I1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -1835,89 +1930,131 @@
       <c r="G2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H3" s="27"/>
+      <c r="K3" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H8" s="28" t="s">
         <v>41</v>
       </c>
+      <c r="I8" s="29" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>